<commit_message>
Update the Capsule List
</commit_message>
<xml_diff>
--- a/Capsule List.xlsx
+++ b/Capsule List.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\ROCapsules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan paplaczyk\Dropbox\GAMES\KSP\Git\ROCapsules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9A95345-3460-4D87-A652-BCB62EB84B5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88590D1B-89B0-4A15-A139-5641570F3989}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mercury" sheetId="6" r:id="rId2"/>
+    <sheet name="Apollo" sheetId="2" r:id="rId3"/>
+    <sheet name="Soyuz" sheetId="3" r:id="rId4"/>
+    <sheet name="VA-TKS" sheetId="4" r:id="rId5"/>
+    <sheet name="Vostok" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="220">
   <si>
     <t>Capsule</t>
   </si>
@@ -81,9 +90,6 @@
     <t>FASA, BDB</t>
   </si>
   <si>
-    <t>FASA, SSTU, BDB</t>
-  </si>
-  <si>
     <t>Airlock</t>
   </si>
   <si>
@@ -124,13 +130,577 @@
   </si>
   <si>
     <t>Modern</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>FASA, SSTU, BDB, DECQ</t>
+  </si>
+  <si>
+    <t>DECQ</t>
+  </si>
+  <si>
+    <t>PART</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Apollo Command Module</t>
+  </si>
+  <si>
+    <t>APOLLO_CM</t>
+  </si>
+  <si>
+    <t>Drogue Parachutes</t>
+  </si>
+  <si>
+    <t>INTERIM.PARACHUTE</t>
+  </si>
+  <si>
+    <t>Forward Heat Shield</t>
+  </si>
+  <si>
+    <t>DOCKInPORT</t>
+  </si>
+  <si>
+    <t>HGA</t>
+  </si>
+  <si>
+    <t>APOLLO_High_Gain_S_band_Antenna</t>
+  </si>
+  <si>
+    <t>LES</t>
+  </si>
+  <si>
+    <t>APOLLO_EAS_TOWER_JETTISON_MOTOR</t>
+  </si>
+  <si>
+    <t>LES Cover</t>
+  </si>
+  <si>
+    <t>APOLLO_EAS_CAP</t>
+  </si>
+  <si>
+    <t>LEM Ascent Stage</t>
+  </si>
+  <si>
+    <t>LEM_ASCENT_STAGE</t>
+  </si>
+  <si>
+    <t>LEM Decoupler</t>
+  </si>
+  <si>
+    <t>LEM_SEPARAT</t>
+  </si>
+  <si>
+    <t>LEM_DESERT_STAGE</t>
+  </si>
+  <si>
+    <t>Lunar Roving Vehicle</t>
+  </si>
+  <si>
+    <t>LRV</t>
+  </si>
+  <si>
+    <t>Main Parachute</t>
+  </si>
+  <si>
+    <t>APOLLO_CHUTE</t>
+  </si>
+  <si>
+    <t>Apollo Service Module</t>
+  </si>
+  <si>
+    <t>APOLLO_SM</t>
+  </si>
+  <si>
+    <t>RCS Block</t>
+  </si>
+  <si>
+    <t>APOLLO_RCS</t>
+  </si>
+  <si>
+    <t>LMDE</t>
+  </si>
+  <si>
+    <t>LEM_D_ENGINE</t>
+  </si>
+  <si>
+    <t>Saturn V Launch Tower</t>
+  </si>
+  <si>
+    <t>TOWER_SV</t>
+  </si>
+  <si>
+    <t>CRAFT</t>
+  </si>
+  <si>
+    <t>LEM</t>
+  </si>
+  <si>
+    <t>Saturn</t>
+  </si>
+  <si>
+    <t>Soyuz 7K Descent Module</t>
+  </si>
+  <si>
+    <t>ok_sa</t>
+  </si>
+  <si>
+    <t>7K Parachute</t>
+  </si>
+  <si>
+    <t>ok_para</t>
+  </si>
+  <si>
+    <t>7K-OK Orbital Module Drogue</t>
+  </si>
+  <si>
+    <t>ok_bo_fem</t>
+  </si>
+  <si>
+    <t>7K-OK Orbital Module Probe</t>
+  </si>
+  <si>
+    <t>ok_bo_male</t>
+  </si>
+  <si>
+    <t>7K-OK Service Module</t>
+  </si>
+  <si>
+    <t>ok_pao</t>
+  </si>
+  <si>
+    <t>7K Decoupler</t>
+  </si>
+  <si>
+    <t>ok_dec</t>
+  </si>
+  <si>
+    <t>7K Toroidal Fuel Tank</t>
+  </si>
+  <si>
+    <t>ok_tft</t>
+  </si>
+  <si>
+    <t>Integrate into bottom of OK SM</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Soyuz Heatshield</t>
+  </si>
+  <si>
+    <t>ok_hs</t>
+  </si>
+  <si>
+    <t>Integrate into bottom of 7K DM</t>
+  </si>
+  <si>
+    <t>7K-OK, 7K-T</t>
+  </si>
+  <si>
+    <t>7K-OK</t>
+  </si>
+  <si>
+    <t>7K-T Orbital Module</t>
+  </si>
+  <si>
+    <t>t_bo</t>
+  </si>
+  <si>
+    <t>7K-T</t>
+  </si>
+  <si>
+    <t>7K Left Solar Array</t>
+  </si>
+  <si>
+    <t>7k_ok_lsolar</t>
+  </si>
+  <si>
+    <t>7K Right Solar Array</t>
+  </si>
+  <si>
+    <t>7k_ok_rsolar</t>
+  </si>
+  <si>
+    <t>7K-T Service Module</t>
+  </si>
+  <si>
+    <t>t_pao</t>
+  </si>
+  <si>
+    <t>7K-T Docking Port</t>
+  </si>
+  <si>
+    <t>t_dp</t>
+  </si>
+  <si>
+    <t>Progress Instrument Module</t>
+  </si>
+  <si>
+    <t>tg_sa</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Progress Orbital Module</t>
+  </si>
+  <si>
+    <t>tg_bo</t>
+  </si>
+  <si>
+    <t>7K-OK, 7K-T, Progress</t>
+  </si>
+  <si>
+    <t>7K-T, Progress</t>
+  </si>
+  <si>
+    <t>7K-LOK Descent Module</t>
+  </si>
+  <si>
+    <t>rn_lok_sa</t>
+  </si>
+  <si>
+    <t>7K-LOK</t>
+  </si>
+  <si>
+    <t>7K-LOK Parachute</t>
+  </si>
+  <si>
+    <t>rn_lok_para</t>
+  </si>
+  <si>
+    <t>7K-LOK Orbital Module</t>
+  </si>
+  <si>
+    <t>rn_lok_bo</t>
+  </si>
+  <si>
+    <t>7K-LOK Service Module</t>
+  </si>
+  <si>
+    <t>rn_lok_tdu</t>
+  </si>
+  <si>
+    <t>7K-LOK Decoupler</t>
+  </si>
+  <si>
+    <t>rn_lok_dec</t>
+  </si>
+  <si>
+    <t>LK Lander Legs</t>
+  </si>
+  <si>
+    <t>rn_lk_lander_legs</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>LK Lander Module</t>
+  </si>
+  <si>
+    <t>rn_lk_lander</t>
+  </si>
+  <si>
+    <t>RD-858</t>
+  </si>
+  <si>
+    <t>rn_lk_rd858</t>
+  </si>
+  <si>
+    <t>RD-859</t>
+  </si>
+  <si>
+    <t>rn_lk_rd859</t>
+  </si>
+  <si>
+    <t>RD-858 Vernier</t>
+  </si>
+  <si>
+    <t>rn_lk_rd858_vernier</t>
+  </si>
+  <si>
+    <t>VA Capsule</t>
+  </si>
+  <si>
+    <t>rn_va_capsule</t>
+  </si>
+  <si>
+    <t>TKS</t>
+  </si>
+  <si>
+    <t>VA Decoupler</t>
+  </si>
+  <si>
+    <t>rn_va_dec</t>
+  </si>
+  <si>
+    <t>VA Parachutes</t>
+  </si>
+  <si>
+    <t>rn_va_para</t>
+  </si>
+  <si>
+    <t>VA RCS</t>
+  </si>
+  <si>
+    <t>rn_tks_va_rcs</t>
+  </si>
+  <si>
+    <t>VA Retro Block</t>
+  </si>
+  <si>
+    <t>rn_tks_retro</t>
+  </si>
+  <si>
+    <t>VA LES</t>
+  </si>
+  <si>
+    <t>rn_va_les</t>
+  </si>
+  <si>
+    <t>TKS Solar Array</t>
+  </si>
+  <si>
+    <t>Kosmos_TKS_Solar_Array_rn</t>
+  </si>
+  <si>
+    <t>TKS RCS</t>
+  </si>
+  <si>
+    <t>rn_tks_rcs_block</t>
+  </si>
+  <si>
+    <t>TKS Supply Craft</t>
+  </si>
+  <si>
+    <t>rn_tks</t>
+  </si>
+  <si>
+    <t>Vostok Descent Module</t>
+  </si>
+  <si>
+    <t>rn_vostok_sc</t>
+  </si>
+  <si>
+    <t>Vostok, Voskhod</t>
+  </si>
+  <si>
+    <t>rn_vostok_dec</t>
+  </si>
+  <si>
+    <t>rn_vostok_tdu</t>
+  </si>
+  <si>
+    <t>Voskhod Descent Module</t>
+  </si>
+  <si>
+    <t>rn_voskhod_sc</t>
+  </si>
+  <si>
+    <t>Voskhod</t>
+  </si>
+  <si>
+    <t>Voskhod Retro Decoupler</t>
+  </si>
+  <si>
+    <t>rn_voskhod_retro_dec</t>
+  </si>
+  <si>
+    <t>Voskhod Retro Package</t>
+  </si>
+  <si>
+    <t>rn_voskhod_retro</t>
+  </si>
+  <si>
+    <t>Voskhod Airlock</t>
+  </si>
+  <si>
+    <t>rn_voskhod_airlock</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>rn_vostok_para</t>
+  </si>
+  <si>
+    <t>Vostok/Voskhod Parachute</t>
+  </si>
+  <si>
+    <t>Vostok/Voskhod Decoupler</t>
+  </si>
+  <si>
+    <t>Vostok/Voskhod Service Module</t>
+  </si>
+  <si>
+    <t>PART NAME</t>
+  </si>
+  <si>
+    <t>ROC-VostokCapsule</t>
+  </si>
+  <si>
+    <t>ROC-VoskhodCapsule</t>
+  </si>
+  <si>
+    <t>ROC-VostokParachute</t>
+  </si>
+  <si>
+    <t>ROC-VostokDecoupler</t>
+  </si>
+  <si>
+    <t>ROC-VostokService</t>
+  </si>
+  <si>
+    <t>ROC-VoskhodRetroDecoupler</t>
+  </si>
+  <si>
+    <t>ROC-VoskhodRetroBooster</t>
+  </si>
+  <si>
+    <t>ROC-VoskhodAirlock</t>
+  </si>
+  <si>
+    <t>LEM Descent Stage-J</t>
+  </si>
+  <si>
+    <t>LEM Descent Stage</t>
+  </si>
+  <si>
+    <t>LEM Docking Port</t>
+  </si>
+  <si>
+    <t>Integrate into Ascent Stage</t>
+  </si>
+  <si>
+    <t>Add Node for them inside CM</t>
+  </si>
+  <si>
+    <t>ROC-ApolloCM</t>
+  </si>
+  <si>
+    <t>ROC-ApolloSM</t>
+  </si>
+  <si>
+    <t>Includes integrated Heat Shield and Drogue Attach</t>
+  </si>
+  <si>
+    <t>ROC-ApolloDroguePara</t>
+  </si>
+  <si>
+    <t>ROC-ApolloForwardHS</t>
+  </si>
+  <si>
+    <t>ROC-ApolloHGA</t>
+  </si>
+  <si>
+    <t>ROC-ApolloLESCover</t>
+  </si>
+  <si>
+    <t>Combined with Pitch Motor</t>
+  </si>
+  <si>
+    <t>ROC-ApolloLES</t>
+  </si>
+  <si>
+    <t>ROC-ApolloParachute</t>
+  </si>
+  <si>
+    <t>Mercury Launch Escape System</t>
+  </si>
+  <si>
+    <t>FASA_Mercury_LES</t>
+  </si>
+  <si>
+    <t>FASAMercuryPodRCS</t>
+  </si>
+  <si>
+    <t>Mercury RCS Thruster Pack</t>
+  </si>
+  <si>
+    <t>FASAMercuryPod</t>
+  </si>
+  <si>
+    <t>Mercury Command Pod</t>
+  </si>
+  <si>
+    <t>FASAMercuryDec</t>
+  </si>
+  <si>
+    <t>Mercury Retro Decoupler</t>
+  </si>
+  <si>
+    <t>Mercury Retro Rocket Pack</t>
+  </si>
+  <si>
+    <t>FASA_Mercury_Eng</t>
+  </si>
+  <si>
+    <t>FASA_Mercury_Parachute_Box</t>
+  </si>
+  <si>
+    <t>Mercury Parachute</t>
+  </si>
+  <si>
+    <t>FASAMercruyCap2</t>
+  </si>
+  <si>
+    <t>ROC-MercuryCM</t>
+  </si>
+  <si>
+    <t>ROC-MercuryLES</t>
+  </si>
+  <si>
+    <t>ROC-MercuryNose</t>
+  </si>
+  <si>
+    <t>ROC-MercuryParachute</t>
+  </si>
+  <si>
+    <t>ROC-MercuryRCS</t>
+  </si>
+  <si>
+    <t>ROC-MercuryRetro</t>
+  </si>
+  <si>
+    <t>ROC-MercuryAdapterRedstone</t>
+  </si>
+  <si>
+    <t>ROC-MercuryAdapterAtlas</t>
+  </si>
+  <si>
+    <t>Mercury Nose Fairing &amp; Antenna</t>
+  </si>
+  <si>
+    <t>ROC-MercuryRetroDecoupler</t>
+  </si>
+  <si>
+    <t>ROC-MercuryPosigrade</t>
+  </si>
+  <si>
+    <t>Mercury-Redstone Adapter</t>
+  </si>
+  <si>
+    <t>Mercury-Atlas Adapter</t>
+  </si>
+  <si>
+    <t>Mercury Posigrade Solid Rocket Motor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +708,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,17 +745,284 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -176,6 +1033,39 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:F11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="PART" dataDxfId="6"/>
+    <tableColumn id="2" name="NAME" dataDxfId="5"/>
+    <tableColumn id="3" name="CRAFT" dataDxfId="4"/>
+    <tableColumn id="4" name="NOTES" dataDxfId="3"/>
+    <tableColumn id="5" name="COMPLETE" dataDxfId="2"/>
+    <tableColumn id="6" name="PART NAME" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18"/>
+  <sortState ref="A2:F18">
+    <sortCondition ref="C1:C18"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="PART"/>
+    <tableColumn id="2" name="NAME"/>
+    <tableColumn id="3" name="CRAFT"/>
+    <tableColumn id="4" name="NOTES"/>
+    <tableColumn id="5" name="COMPLETE" dataDxfId="0"/>
+    <tableColumn id="6" name="PART NAME"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,11 +1364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638335AD-E989-4510-92B6-2D87A171C345}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +1430,12 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -549,7 +1445,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -563,10 +1459,10 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -574,94 +1470,1196 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
+        <v>68</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>